<commit_message>
Alterações finais - 01/06
</commit_message>
<xml_diff>
--- a/17 - Análises de Eventos/Análise - Alocação de Local para Eventos + Venda de ingressos.xlsx
+++ b/17 - Análises de Eventos/Análise - Alocação de Local para Eventos + Venda de ingressos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t xml:space="preserve">Capacidades </t>
   </si>
@@ -52,31 +52,28 @@
     <t>FB</t>
   </si>
   <si>
-    <t>Associado avalia local do evento</t>
+    <t>Associado procura por local do evento</t>
   </si>
   <si>
     <t>x</t>
   </si>
   <si>
-    <t>Associado agenda evento</t>
+    <t>Associado negocia local evento</t>
   </si>
   <si>
     <t>x(1)</t>
   </si>
   <si>
-    <t>Associados divulgam evento</t>
+    <t>Associado divulga evento</t>
   </si>
   <si>
     <t>x(2)</t>
   </si>
   <si>
-    <t>Associados organizam local do evento</t>
-  </si>
-  <si>
     <t>FA</t>
   </si>
   <si>
-    <t>Associado cancela evento</t>
+    <t>Associado cancela locação</t>
   </si>
   <si>
     <t>Venda de ingressos</t>
@@ -91,7 +88,7 @@
     <t>Associado vende ingressos</t>
   </si>
   <si>
-    <t>x(6)</t>
+    <t>x(5)</t>
   </si>
 </sst>
 </file>
@@ -162,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border/>
     <border>
       <left style="thin">
@@ -279,17 +276,12 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="41">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -350,18 +342,6 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="5" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -383,29 +363,17 @@
     <xf borderId="13" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="10" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
@@ -748,166 +716,97 @@
       <c r="K5" s="6"/>
     </row>
     <row r="6">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
+      <c r="A6" s="12"/>
+      <c r="B6" s="20" t="s">
+        <v>19</v>
+      </c>
       <c r="C6" s="17">
         <v>4.0</v>
       </c>
-      <c r="D6" s="25" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27" t="s">
+      <c r="D6" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="17"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="28"/>
-      <c r="K6" s="2"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="6"/>
     </row>
     <row r="7">
-      <c r="A7" s="22"/>
-      <c r="B7" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="27">
+      <c r="A7" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="26">
         <v>5.0</v>
       </c>
-      <c r="D7" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="J7" s="21"/>
-      <c r="K7" s="6"/>
+      <c r="D7" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="28"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="31"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8">
-      <c r="A8" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>12</v>
-      </c>
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="30">
         <v>6.0</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="32"/>
+      <c r="D8" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="31"/>
       <c r="F8" s="33"/>
-      <c r="G8" s="34" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="35"/>
-      <c r="I8" s="32"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="12"/>
-      <c r="B9" s="12"/>
-      <c r="C9" s="37">
-        <v>7.0</v>
-      </c>
-      <c r="D9" s="38" t="s">
+      <c r="G8" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="H9" s="40"/>
-      <c r="I9" s="40"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="23"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="43"/>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="11">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-      <c r="H11" s="45"/>
-      <c r="I11" s="45"/>
-      <c r="J11" s="45"/>
-      <c r="K11" s="45"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="44"/>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="45"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45"/>
-      <c r="C13" s="45"/>
-      <c r="D13" s="45"/>
-      <c r="E13" s="45"/>
-      <c r="F13" s="45"/>
-      <c r="G13" s="45"/>
-      <c r="H13" s="45"/>
-      <c r="I13" s="45"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="45"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="36"/>
+      <c r="I11" s="36"/>
+      <c r="J11" s="36"/>
+      <c r="K11" s="36"/>
     </row>
     <row r="14">
-      <c r="A14" s="44"/>
-      <c r="B14" s="42"/>
-      <c r="C14" s="46"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="46"/>
-      <c r="H14" s="47"/>
-      <c r="I14" s="46"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="39"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="38"/>
     </row>
     <row r="18">
-      <c r="F18" s="48"/>
+      <c r="F18" s="40"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:I1"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="J14:K14"/>
+  <mergeCells count="17">
     <mergeCell ref="J1:K2"/>
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="J4:K4"/>
@@ -915,6 +814,16 @@
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="B3:B5"/>
   </mergeCells>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>